<commit_message>
feat: Phase 10 — enterprise-readiness features
- build_all_domains(): auto-orders domains (DM first), passes dm_data downstream
- SELECT column filtering: metadata files support optional select='Y' column
  for study-specific subsetting from global metadata templates
- create_supp toggle: new param on build_domain(), build_all_domains(), and
  new_sdtm_config(); set FALSE to keep all vars in main domain (no SUPP--)
- Extra columns in metadata files are silently tolerated (backward compatible)
- Starter kit CSV/XLSX updated with select column
- check_end_to_end and demo_full_pipeline refactored to use build_all_domains()
- README updated with new features, SELECT docs, build_all_domains examples
- NEWS.md updated with Phase 9 + Phase 10 changelogs
- Removed stale ROADMAP.md

289 tests passing, 10/10 domains build with 0 errors.
</commit_message>
<xml_diff>
--- a/inst/extdata/starter_kit/ct_codelist.xlsx
+++ b/inst/extdata/starter_kit/ct_codelist.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,35 +360,40 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>select</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>codelist_id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>codelist_name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>input_value</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>coded_value</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>decode</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>case_sensitive</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
@@ -397,35 +402,40 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>C66769</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Severity/Intensity Scale for Adverse Events</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>mild</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>MILD</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Mild</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
         <is>
           <t>AESEV</t>
         </is>
@@ -434,35 +444,40 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>C66769</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Severity/Intensity Scale for Adverse Events</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>moderate</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>MODERATE</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Moderate</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G3" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>AESEV</t>
         </is>
@@ -471,35 +486,40 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>C66769</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Severity/Intensity Scale for Adverse Events</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>severe</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>SEVERE</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G4" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>AESEV</t>
         </is>
@@ -508,35 +528,40 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>C66769</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Severity/Intensity Scale for Adverse Events</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>MILD</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>MILD</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Mild</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G5" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
         <is>
           <t>AESEV uppercase</t>
         </is>
@@ -545,35 +570,40 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>C66769</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Severity/Intensity Scale for Adverse Events</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>MODERATE</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>MODERATE</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>Moderate</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G6" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
         <is>
           <t>AESEV uppercase</t>
         </is>
@@ -582,35 +612,40 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>C66769</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Severity/Intensity Scale for Adverse Events</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>SEVERE</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>SEVERE</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G7" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
         <is>
           <t>AESEV uppercase</t>
         </is>
@@ -619,35 +654,40 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>C66769</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Severity/Intensity Scale for Adverse Events</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Mild</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>MILD</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>Mild</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G8" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
         <is>
           <t>AESEV mixed case</t>
         </is>
@@ -656,35 +696,40 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>C66769</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>Severity/Intensity Scale for Adverse Events</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Moderate</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>MODERATE</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>Moderate</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G9" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
         <is>
           <t>AESEV mixed case</t>
         </is>
@@ -693,35 +738,40 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>C66769</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>Severity/Intensity Scale for Adverse Events</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>SEVERE</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G10" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
         <is>
           <t>AESEV mixed case</t>
         </is>
@@ -730,35 +780,40 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>C66770</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>Causality</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>related</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>RELATED</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>Related</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G11" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
         <is>
           <t>AEREL</t>
         </is>
@@ -767,35 +822,40 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>C66770</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>Causality</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>not related</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>NOT RELATED</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>Not Related</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G12" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
         <is>
           <t>AEREL</t>
         </is>
@@ -804,35 +864,40 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>C66770</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>Causality</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>possibly related</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>POSSIBLY RELATED</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>Possibly Related</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G13" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
         <is>
           <t>AEREL</t>
         </is>
@@ -841,35 +906,40 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>C66770</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>Causality</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>RELATED</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>RELATED</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>Related</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G14" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
         <is>
           <t>AEREL uppercase</t>
         </is>
@@ -878,35 +948,40 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>C66770</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>Causality</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>NOT RELATED</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>NOT RELATED</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>Not Related</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G15" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
         <is>
           <t>AEREL uppercase</t>
         </is>
@@ -915,35 +990,40 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>C66770</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>Causality</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>POSSIBLY RELATED</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>POSSIBLY RELATED</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>Possibly Related</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G16" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
         <is>
           <t>AEREL uppercase</t>
         </is>
@@ -952,35 +1032,40 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>YN</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>Yes/No Response</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="E17" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G17" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
         <is>
           <t>generic Y/N</t>
         </is>
@@ -989,35 +1074,40 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>YN</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>Yes/No Response</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>n</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="E18" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G18" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
         <is>
           <t>generic Y/N</t>
         </is>
@@ -1026,19 +1116,19 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>YN</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>Yes/No Response</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="D19" t="inlineStr">
         <is>
           <t>Y</t>
@@ -1046,15 +1136,20 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G19" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
         <is>
           <t>generic Y/N uppercase</t>
         </is>
@@ -1063,19 +1158,19 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>YN</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>Yes/No Response</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="D20" t="inlineStr">
         <is>
           <t>N</t>
@@ -1083,15 +1178,20 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G20" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
         <is>
           <t>generic Y/N uppercase</t>
         </is>
@@ -1100,35 +1200,40 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>YN</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>Yes/No Response</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="E21" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G21" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
         <is>
           <t>generic Y/N</t>
         </is>
@@ -1137,35 +1242,40 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
           <t>YN</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>Yes/No Response</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="E22" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G22" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
         <is>
           <t>generic Y/N</t>
         </is>
@@ -1174,35 +1284,40 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>ROUTE</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>Route of Administration</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>oral</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>ORAL</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>Oral</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G23" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
         <is>
           <t>CMROUTE</t>
         </is>
@@ -1211,35 +1326,40 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>ROUTE</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>Route of Administration</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>iv</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>INTRAVENOUS</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>Intravenous</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G24" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
         <is>
           <t>CMROUTE</t>
         </is>
@@ -1248,35 +1368,40 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
           <t>ROUTE</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>Route of Administration</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>topical</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>TOPICAL</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>Topical</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G25" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
         <is>
           <t>CMROUTE</t>
         </is>
@@ -1285,35 +1410,40 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t>ROUTE</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>Route of Administration</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>ORAL</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>ORAL</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>Oral</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G26" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
         <is>
           <t>CMROUTE uppercase</t>
         </is>
@@ -1322,35 +1452,40 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
           <t>ROUTE</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>Route of Administration</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>INTRAVENOUS</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>INTRAVENOUS</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>Intravenous</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G27" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
         <is>
           <t>CMROUTE</t>
         </is>
@@ -1359,35 +1494,40 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>ROUTE</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>Route of Administration</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>subcutaneous</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>SUBCUTANEOUS</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>Subcutaneous</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G28" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
         <is>
           <t>CMROUTE</t>
         </is>
@@ -1396,35 +1536,40 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>UNIT</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>Unit</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>mg</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>mg</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>mg</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="G29" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
         <is>
           <t>dose units</t>
         </is>
@@ -1433,35 +1578,40 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
           <t>UNIT</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>Unit</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>ml</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>mL</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>mL</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G30" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
         <is>
           <t>dose units</t>
         </is>
@@ -1470,35 +1620,40 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>UNIT</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="C31" t="inlineStr">
         <is>
           <t>Unit</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>g</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>g</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="F31" t="inlineStr">
         <is>
           <t>g</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="G31" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
         <is>
           <t>dose units</t>
         </is>
@@ -1507,35 +1662,40 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
           <t>UNIT</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>Unit</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>mcg</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>mcg</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>mcg</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="G32" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
         <is>
           <t>dose units</t>
         </is>
@@ -1544,35 +1704,40 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
           <t>FREQ</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>qd</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>QD</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>Every Day</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G33" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
         <is>
           <t>CMDOSFRQ</t>
         </is>
@@ -1581,35 +1746,40 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
           <t>FREQ</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>bid</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>BID</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>Twice a Day</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G34" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
         <is>
           <t>CMDOSFRQ</t>
         </is>
@@ -1618,35 +1788,40 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
           <t>FREQ</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>tid</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>TID</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="F35" t="inlineStr">
         <is>
           <t>Three Times a Day</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G35" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
         <is>
           <t>CMDOSFRQ</t>
         </is>
@@ -1655,35 +1830,40 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
           <t>FREQ</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>prn</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t>PRN</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="F36" t="inlineStr">
         <is>
           <t>As Needed</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G36" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
         <is>
           <t>CMDOSFRQ</t>
         </is>
@@ -1692,35 +1872,40 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
           <t>FREQ</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>QD</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>QD</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="F37" t="inlineStr">
         <is>
           <t>Every Day</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G37" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
         <is>
           <t>CMDOSFRQ uppercase</t>
         </is>
@@ -1729,35 +1914,40 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
           <t>FREQ</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>BID</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t>BID</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>Twice a Day</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G38" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
         <is>
           <t>CMDOSFRQ uppercase</t>
         </is>
@@ -1766,35 +1956,40 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
           <t>SEX</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="C39" t="inlineStr">
         <is>
           <t>Sex</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="E39" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G39" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
         <is>
           <t>DM SEX</t>
         </is>
@@ -1803,35 +1998,40 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
           <t>SEX</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>Sex</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G40" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
         <is>
           <t>DM SEX</t>
         </is>
@@ -1840,35 +2040,40 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
           <t>SEX</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="C41" t="inlineStr">
         <is>
           <t>Sex</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>m</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="F41" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G41" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
         <is>
           <t>DM SEX lowercase</t>
         </is>
@@ -1877,35 +2082,40 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
           <t>SEX</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>Sex</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>f</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
+      <c r="F42" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G42" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
         <is>
           <t>DM SEX lowercase</t>
         </is>
@@ -1914,35 +2124,40 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
           <t>RACE</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>Race</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>WHITE</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="E43" t="inlineStr">
         <is>
           <t>WHITE</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="F43" t="inlineStr">
         <is>
           <t>White</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G43" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
         <is>
           <t>DM RACE</t>
         </is>
@@ -1951,35 +2166,40 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
           <t>RACE</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>Race</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>BLACK OR AFRICAN AMERICAN</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="E44" t="inlineStr">
         <is>
           <t>BLACK OR AFRICAN AMERICAN</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="F44" t="inlineStr">
         <is>
           <t>Black or African American</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G44" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
         <is>
           <t>DM RACE</t>
         </is>
@@ -1988,35 +2208,40 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
           <t>RACE</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="C45" t="inlineStr">
         <is>
           <t>Race</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>ASIAN</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="E45" t="inlineStr">
         <is>
           <t>ASIAN</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="F45" t="inlineStr">
         <is>
           <t>Asian</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G45" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
         <is>
           <t>DM RACE</t>
         </is>
@@ -2025,35 +2250,40 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
           <t>RACE</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>Race</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>OTHER</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>OTHER</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="F46" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G46" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
         <is>
           <t>DM RACE</t>
         </is>
@@ -2062,35 +2292,40 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
           <t>RACE</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="C47" t="inlineStr">
         <is>
           <t>Race</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t>white</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="E47" t="inlineStr">
         <is>
           <t>WHITE</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="F47" t="inlineStr">
         <is>
           <t>White</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G47" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
         <is>
           <t>DM RACE lowercase</t>
         </is>
@@ -2099,35 +2334,40 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
           <t>RACE</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="C48" t="inlineStr">
         <is>
           <t>Race</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>asian</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>ASIAN</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
+      <c r="F48" t="inlineStr">
         <is>
           <t>Asian</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G48" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
         <is>
           <t>DM RACE lowercase</t>
         </is>
@@ -2136,35 +2376,40 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
           <t>AGEU</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>Age Unit</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>YEARS</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="E49" t="inlineStr">
         <is>
           <t>YEARS</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
+      <c r="F49" t="inlineStr">
         <is>
           <t>Years</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G49" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
         <is>
           <t>DM AGEU</t>
         </is>
@@ -2173,35 +2418,40 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
           <t>AGEU</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="C50" t="inlineStr">
         <is>
           <t>Age Unit</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>years</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="E50" t="inlineStr">
         <is>
           <t>YEARS</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
+      <c r="F50" t="inlineStr">
         <is>
           <t>Years</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G50" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
         <is>
           <t>DM AGEU lowercase</t>
         </is>
@@ -2210,35 +2460,40 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
           <t>AGEU</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="C51" t="inlineStr">
         <is>
           <t>Age Unit</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>Years</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t>YEARS</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="F51" t="inlineStr">
         <is>
           <t>Years</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G51" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
         <is>
           <t>DM AGEU mixed</t>
         </is>
@@ -2247,35 +2502,40 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
           <t>QSTEST</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>Questionnaire Test Name</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="D52" t="inlineStr">
         <is>
           <t>FUNC01</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>FUNC01</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
+      <c r="F52" t="inlineStr">
         <is>
           <t>Physical Functioning Score</t>
         </is>
       </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G52" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
         <is>
           <t>QS decode</t>
         </is>
@@ -2284,35 +2544,40 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
           <t>QSTEST</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="C53" t="inlineStr">
         <is>
           <t>Questionnaire Test Name</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="D53" t="inlineStr">
         <is>
           <t>FUNC02</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="E53" t="inlineStr">
         <is>
           <t>FUNC02</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
+      <c r="F53" t="inlineStr">
         <is>
           <t>Emotional Well-Being Score</t>
         </is>
       </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G53" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
         <is>
           <t>QS decode</t>
         </is>
@@ -2321,35 +2586,40 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
           <t>QSTEST</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="C54" t="inlineStr">
         <is>
           <t>Questionnaire Test Name</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="D54" t="inlineStr">
         <is>
           <t>FUNC03</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="E54" t="inlineStr">
         <is>
           <t>FUNC03</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
+      <c r="F54" t="inlineStr">
         <is>
           <t>Pain Interference Score</t>
         </is>
       </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
       <c r="G54" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
         <is>
           <t>QS decode</t>
         </is>

</xml_diff>